<commit_message>
create template for future use by steve
</commit_message>
<xml_diff>
--- a/data-raw/bybox_2025_template.xlsx
+++ b/data-raw/bybox_2025_template.xlsx
@@ -1,113 +1,106 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Git/kestrelbox/data-raw/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C799584B-A521-F642-8A7A-746219E3D1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="2660" windowWidth="21180" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="bybox_2025" sheetId="1" r:id="rId1"/>
+    <sheet name="bybox_2025" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
-  <si>
-    <t>box_id</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>did_not_check</t>
-  </si>
-  <si>
-    <t>occupied</t>
-  </si>
-  <si>
-    <t>failure</t>
-  </si>
-  <si>
-    <t>young_count</t>
-  </si>
-  <si>
-    <t>young_count_2nd_brood</t>
-  </si>
-  <si>
-    <t>unbanded_young_count</t>
-  </si>
-  <si>
-    <t>mount_type</t>
-  </si>
-  <si>
-    <t>study_area</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>EXAMPLE1</t>
-  </si>
-  <si>
-    <t>steel pole</t>
-  </si>
-  <si>
-    <t>Central PA</t>
-  </si>
-  <si>
-    <t>EXAMPLE30</t>
-  </si>
-  <si>
-    <t>private u-pole</t>
-  </si>
-  <si>
-    <t>EXAMPLE3</t>
-  </si>
-  <si>
-    <t>EXAMPLE10</t>
-  </si>
-  <si>
-    <t>public u-pole</t>
-  </si>
-  <si>
-    <t>EXAMPLE14</t>
-  </si>
-  <si>
-    <t>EXAMPLE24</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>EXAMPLE308</t>
-  </si>
-  <si>
-    <t>Lancaster</t>
-  </si>
-  <si>
-    <t>EXAMPLE321</t>
-  </si>
-  <si>
-    <t>NJ</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+  <si>
+    <t xml:space="preserve">box_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">did_not_check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">failure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">young_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">young_count_2nd_brood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unbanded_young_count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mount_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">steel pole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central PA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private u-pole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public u-pole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lancaster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXAMPLE321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,17 +109,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <b/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -168,15 +159,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -458,16 +440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:L9"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,23 +485,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>3</v>
       </c>
       <c r="G2" s="2"/>
@@ -532,30 +512,30 @@
       <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="2">
-        <v>41.037967014183302</v>
-      </c>
-      <c r="L2" s="2">
+      <c r="K2" s="2" t="n">
+        <v>41.0379670141833</v>
+      </c>
+      <c r="L2" s="2" t="n">
         <v>-77.6674654697714</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G3" s="2"/>
@@ -566,30 +546,30 @@
       <c r="J3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="2">
-        <v>40.977574711777798</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="K3" s="2" t="n">
+        <v>40.9775747117778</v>
+      </c>
+      <c r="L3" s="2" t="n">
         <v>-77.5846699908912</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="C4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="2"/>
@@ -598,30 +578,30 @@
       <c r="J4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="2" t="n">
         <v>41.0246696443769</v>
       </c>
-      <c r="L4" s="2">
-        <v>-77.456002712104706</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L4" s="2" t="n">
+        <v>-77.4560027121047</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="2"/>
@@ -632,30 +612,30 @@
       <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="2">
-        <v>40.664426488579799</v>
-      </c>
-      <c r="L5" s="2">
-        <v>-77.799380069381201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K5" s="2" t="n">
+        <v>40.6644264885798</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>-77.7993800693812</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
@@ -666,165 +646,275 @@
       <c r="J6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="2">
-        <v>40.490848361801604</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-77.984542632196195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="K6" s="2" t="n">
+        <v>40.4908483618016</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>-77.9845426321962</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="n">
         <v>2024</v>
       </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="2">
-        <v>40.573459141028103</v>
-      </c>
-      <c r="L7" s="2">
-        <v>-78.047547692701201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="K7" t="n">
+        <v>40.5734591410281</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-78.0475476927012</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="n">
         <v>2024</v>
       </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2">
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
         <v>5</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="2">
-        <v>39.971724360792997</v>
-      </c>
-      <c r="L8" s="2">
-        <v>-75.977662199582397</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="K8" t="n">
+        <v>39.971724360793</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-75.9776621995824</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="n">
         <v>2024</v>
       </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="2">
-        <v>39.390264278352703</v>
-      </c>
-      <c r="L9" s="2">
-        <v>-75.325939867450998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="K9" t="n">
+        <v>39.3902642783527</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-75.325939867451</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10"/>
+      <c r="B10" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11">
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11">
+      <c r="A11"/>
+      <c r="B11" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12">
+      <c r="A12"/>
+      <c r="B12" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+    </row>
+    <row r="13">
+      <c r="A13"/>
+      <c r="B13" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B14">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+    </row>
+    <row r="14">
+      <c r="A14"/>
+      <c r="B14" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+    </row>
+    <row r="15">
+      <c r="A15"/>
+      <c r="B15" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+    </row>
+    <row r="16">
+      <c r="A16"/>
+      <c r="B16" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17">
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+    </row>
+    <row r="18">
+      <c r="A18"/>
+      <c r="B18" t="n">
         <v>2025</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19">
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+    </row>
+    <row r="19">
+      <c r="A19"/>
+      <c r="B19" t="n">
         <v>2025</v>
       </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>